<commit_message>
stable edits, we are now adding mouse processing pipeline
</commit_message>
<xml_diff>
--- a/Data_Processing_Notes.xlsx
+++ b/Data_Processing_Notes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wm5wt/Google Drive/UVA/Grad School/Projects/PlaqView_Preprocess/PlaqView_DataProcessing/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wm5wt/Google Drive/UVA/Grad School/Projects/PlaqView/DataProcessing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94E5099E-1185-EE41-9902-3CCB396E2C73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE544A6B-B672-4F44-A6E5-F158D84B2F91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2800" yWindow="700" windowWidth="26000" windowHeight="16940" xr2:uid="{5C0CB6DF-74F5-E84F-91BF-65048458DE00}"/>
+    <workbookView xWindow="0" yWindow="8100" windowWidth="26000" windowHeight="16940" xr2:uid="{5C0CB6DF-74F5-E84F-91BF-65048458DE00}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="28">
   <si>
     <t>DataID</t>
   </si>
@@ -88,6 +88,27 @@
   </si>
   <si>
     <t>Pan_2021_mouse.rds</t>
+  </si>
+  <si>
+    <t>Alencar et al.</t>
+  </si>
+  <si>
+    <t>This is from Gabe Alencar: mouse genome was converted to human, genes were removed (non 1:1 homologues), and then all the libraries were integrated, etc</t>
+  </si>
+  <si>
+    <t>Aencar_2020_mouse.rds</t>
+  </si>
+  <si>
+    <t>Alencar_2020_humanized_homolog</t>
+  </si>
+  <si>
+    <t>Alencar_2020_mouse</t>
+  </si>
+  <si>
+    <t>Aencar_2020_humanized.rds</t>
+  </si>
+  <si>
+    <t>This is from Katie Owsiany: unconverted original mouse data</t>
   </si>
 </sst>
 </file>
@@ -447,16 +468,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAE4BB4F-B325-9D4C-92D3-781BA71EF3E2}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11.1640625" customWidth="1"/>
-    <col min="2" max="2" width="14.33203125" customWidth="1"/>
+    <col min="2" max="2" width="22" customWidth="1"/>
     <col min="3" max="3" width="18.6640625" customWidth="1"/>
     <col min="4" max="4" width="17" customWidth="1"/>
   </cols>
@@ -557,6 +578,40 @@
         <v>17</v>
       </c>
     </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8" t="s">
+        <v>27</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>